<commit_message>
Made graphs comparing the recall and spec of the real world predictions for the 3 model splits. code saved to Thesis Methods.py
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/Forecasting/COVID Impact Forecast Results.xlsx
+++ b/Jeremy Thesis/Forecasting/COVID Impact Forecast Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B9D531-633A-4A62-80D6-7C7E05D606DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4BF0B9-4314-40B6-9D09-35B341507886}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFD92964-F7FE-4639-8012-1C33CD9CC157}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>TP</t>
   </si>
@@ -112,6 +112,39 @@
   </si>
   <si>
     <t>TS 5050 FS T1 6-6-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 1-15-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 1-16-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 1-17-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 1-18-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-12-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-13-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-14-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-15-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-16-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-17-2020</t>
+  </si>
+  <si>
+    <t>TS 5050 FS T1 4-18-2020</t>
   </si>
 </sst>
 </file>
@@ -135,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +190,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -201,12 +246,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -515,19 +571,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930CC131-93F4-46C3-89CE-5D3E42305E11}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1036,6 +1091,328 @@
         <v>0.86671015438138699</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="13">
+        <v>62</v>
+      </c>
+      <c r="C23" s="13">
+        <v>56</v>
+      </c>
+      <c r="D23" s="13">
+        <v>3971</v>
+      </c>
+      <c r="E23" s="13">
+        <v>510</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0.52542372881355903</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0.88618611916982803</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="13">
+        <v>45</v>
+      </c>
+      <c r="C24" s="13">
+        <v>69</v>
+      </c>
+      <c r="D24" s="13">
+        <v>3774</v>
+      </c>
+      <c r="E24" s="13">
+        <v>711</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.394736842105263</v>
+      </c>
+      <c r="G24" s="14">
+        <v>0.84147157190635402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="13">
+        <v>75</v>
+      </c>
+      <c r="C25" s="13">
+        <v>24</v>
+      </c>
+      <c r="D25" s="13">
+        <v>3715</v>
+      </c>
+      <c r="E25" s="13">
+        <v>785</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0.75757575757575701</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0.82555555555555504</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="13">
+        <v>49</v>
+      </c>
+      <c r="C26" s="13">
+        <v>38</v>
+      </c>
+      <c r="D26" s="13">
+        <v>3868</v>
+      </c>
+      <c r="E26" s="13">
+        <v>644</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.56321839080459701</v>
+      </c>
+      <c r="G26" s="14">
+        <v>0.85726950354609899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="13">
+        <v>46</v>
+      </c>
+      <c r="C27" s="13">
+        <v>15</v>
+      </c>
+      <c r="D27" s="13">
+        <v>3973</v>
+      </c>
+      <c r="E27" s="13">
+        <v>565</v>
+      </c>
+      <c r="F27" s="14">
+        <v>0.75409836065573699</v>
+      </c>
+      <c r="G27" s="14">
+        <v>0.87549581313353897</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="13">
+        <v>53</v>
+      </c>
+      <c r="C28" s="13">
+        <v>31</v>
+      </c>
+      <c r="D28" s="13">
+        <v>3810</v>
+      </c>
+      <c r="E28" s="13">
+        <v>705</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.63095238095238004</v>
+      </c>
+      <c r="G28" s="14">
+        <v>0.84385382059800595</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="13">
+        <v>84</v>
+      </c>
+      <c r="C29" s="13">
+        <v>75</v>
+      </c>
+      <c r="D29" s="13">
+        <v>3907</v>
+      </c>
+      <c r="E29" s="13">
+        <v>533</v>
+      </c>
+      <c r="F29" s="14">
+        <v>0.52830188679245205</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0.87995495495495402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="16">
+        <v>23</v>
+      </c>
+      <c r="C30" s="16">
+        <v>55</v>
+      </c>
+      <c r="D30" s="16">
+        <v>3981</v>
+      </c>
+      <c r="E30" s="16">
+        <v>540</v>
+      </c>
+      <c r="F30" s="17">
+        <v>0.29487179487179399</v>
+      </c>
+      <c r="G30" s="17">
+        <v>0.88055739880557404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="16">
+        <v>56</v>
+      </c>
+      <c r="C31" s="16">
+        <v>66</v>
+      </c>
+      <c r="D31" s="16">
+        <v>3849</v>
+      </c>
+      <c r="E31" s="16">
+        <v>628</v>
+      </c>
+      <c r="F31" s="17">
+        <v>0.45901639344262202</v>
+      </c>
+      <c r="G31" s="17">
+        <v>0.85972749609113197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="16">
+        <v>29</v>
+      </c>
+      <c r="C32" s="16">
+        <v>22</v>
+      </c>
+      <c r="D32" s="16">
+        <v>3788</v>
+      </c>
+      <c r="E32" s="16">
+        <v>760</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0.56862745098039202</v>
+      </c>
+      <c r="G32" s="17">
+        <v>0.83289357959542598</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="16">
+        <v>29</v>
+      </c>
+      <c r="C33" s="16">
+        <v>12</v>
+      </c>
+      <c r="D33" s="16">
+        <v>3656</v>
+      </c>
+      <c r="E33" s="16">
+        <v>902</v>
+      </c>
+      <c r="F33" s="17">
+        <v>0.707317073170731</v>
+      </c>
+      <c r="G33" s="17">
+        <v>0.80210618692408897</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="16">
+        <v>40</v>
+      </c>
+      <c r="C34" s="16">
+        <v>27</v>
+      </c>
+      <c r="D34" s="16">
+        <v>3907</v>
+      </c>
+      <c r="E34" s="16">
+        <v>625</v>
+      </c>
+      <c r="F34" s="17">
+        <v>0.59701492537313405</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0.86209179170344197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="16">
+        <v>39</v>
+      </c>
+      <c r="C35" s="16">
+        <v>15</v>
+      </c>
+      <c r="D35" s="16">
+        <v>3755</v>
+      </c>
+      <c r="E35" s="16">
+        <v>790</v>
+      </c>
+      <c r="F35" s="17">
+        <v>0.72222222222222199</v>
+      </c>
+      <c r="G35" s="17">
+        <v>0.82618261826182604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="16">
+        <v>21</v>
+      </c>
+      <c r="C36" s="16">
+        <v>33</v>
+      </c>
+      <c r="D36" s="16">
+        <v>3836</v>
+      </c>
+      <c r="E36" s="16">
+        <v>709</v>
+      </c>
+      <c r="F36" s="17">
+        <v>0.38888888888888801</v>
+      </c>
+      <c r="G36" s="17">
+        <v>0.84400440044004399</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>